<commit_message>
Still working on lab 2 just need to comment the code and add to the excel file.
</commit_message>
<xml_diff>
--- a/nstarklab2/CS361Lab2.xlsx
+++ b/nstarklab2/CS361Lab2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9FF432-65C5-4B67-8A4C-16E3DB199BDC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596001E8-D37E-4FF8-BDB6-46058B1B6C06}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
   <si>
     <t>1 to 1000</t>
   </si>
@@ -53,18 +53,6 @@
   </si>
   <si>
     <t>Quick sort</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
   <si>
     <t>ave. of 1 to 1000</t>
@@ -135,1008 +123,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>1st</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Run</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>of all 5 runs.</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Bin sort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1 to 1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1 to 10000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1 to 100000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1 to 1000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1 to 10000000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>32450497</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>28636922</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>34032187</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>53449699</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>182235238</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0301-471D-BBF9-D4B95F19D918}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Radix sort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1 to 1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1 to 10000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1 to 100000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1 to 1000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1 to 10000000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>637358</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3018010</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15717967</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>103563842</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1047301160</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0301-471D-BBF9-D4B95F19D918}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Quick sort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1 to 1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1 to 10000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1 to 100000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1 to 1000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1 to 10000000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$2:$D$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>454231</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1775767</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12404311</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>94535488</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2090318656</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-0301-471D-BBF9-D4B95F19D918}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="471695872"/>
-        <c:axId val="342419080"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="471695872"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="342419080"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="342419080"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="471695872"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>1st 4 runs of 1st Run</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Bin sort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1 to 1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1 to 10000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1 to 100000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1 to 1000000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>32450497</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>28636922</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>34032187</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>53449699</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-04A0-4702-AD21-17619897EB64}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Radix sort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1 to 1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1 to 10000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1 to 100000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1 to 1000000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>637358</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3018010</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15717967</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>103563842</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-04A0-4702-AD21-17619897EB64}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Quick sort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1 to 1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1 to 10000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1 to 100000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1 to 1000000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$2:$D$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>454231</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1775767</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12404311</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>94535488</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-04A0-4702-AD21-17619897EB64}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="344327440"/>
-        <c:axId val="344327768"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="344327440"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="344327768"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="344327768"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="344327440"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1639,7 +625,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2204,86 +1190,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3290,1086 +2196,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>320675</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>15875</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFEBF73B-59A8-480C-BAAE-1AB3EFD87B79}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>415925</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>111125</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{394797EA-7E2A-41EF-8373-7A3D4C4A60EC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -4400,7 +2228,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4436,7 +2264,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4710,8 +2538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4987,7 +2815,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B25">
         <f>AVERAGE(B16,B9,B2)</f>
@@ -5004,7 +2832,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B27">
         <f>AVERAGE(D3,D10,D17)</f>
@@ -5021,7 +2849,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B29">
         <f>AVERAGE(D18,D11,D4)</f>
@@ -5038,7 +2866,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B31">
         <f>AVERAGE(D19,D12,D5)</f>
@@ -5055,7 +2883,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B33">
         <f>AVERAGE(D20,D13,D6)</f>

</xml_diff>